<commit_message>
Fix generate XBRL Form nihil.
</commit_message>
<xml_diff>
--- a/templates/tmp_ls10.xlsx
+++ b/templates/tmp_ls10.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Rekening" sheetId="1" r:id="rId1"/>
+    <sheet name="Agunan" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="70">
   <si>
     <t>NOMOR_NASABAH</t>
   </si>
@@ -125,6 +126,105 @@
   </si>
   <si>
     <t>CKPN_KOLEKTIF</t>
+  </si>
+  <si>
+    <t>111111</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7  </t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">9 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5   </t>
+  </si>
+  <si>
+    <t>888888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4  </t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">7         </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2   </t>
+  </si>
+  <si>
+    <t>JENIS_ASSET</t>
+  </si>
+  <si>
+    <t>NO_AGUNAN</t>
+  </si>
+  <si>
+    <t>SIFAT_AGUNAN</t>
+  </si>
+  <si>
+    <t>GOLONGAN_PENERBIT</t>
+  </si>
+  <si>
+    <t>TGL_PENILAIAN</t>
+  </si>
+  <si>
+    <t>NILAI_AGUNAN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3  </t>
   </si>
 </sst>
 </file>
@@ -473,7 +573,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AK1"/>
+  <dimension ref="A1:AK3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,6 +731,415 @@
         <v>36</v>
       </c>
     </row>
+    <row r="2" spans="1:37">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K2" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>40</v>
+      </c>
+      <c r="O2" t="s">
+        <v>41</v>
+      </c>
+      <c r="P2" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
+        <v>39</v>
+      </c>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Y2">
+        <v>5</v>
+      </c>
+      <c r="Z2">
+        <v>6</v>
+      </c>
+      <c r="AA2">
+        <v>7</v>
+      </c>
+      <c r="AB2">
+        <v>8</v>
+      </c>
+      <c r="AC2">
+        <v>9</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>2</v>
+      </c>
+      <c r="AG2">
+        <v>3</v>
+      </c>
+      <c r="AH2">
+        <v>4</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AJ2">
+        <v>6</v>
+      </c>
+      <c r="AK2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N3" t="s">
+        <v>47</v>
+      </c>
+      <c r="O3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>57</v>
+      </c>
+      <c r="R3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U3">
+        <v>8</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" t="s">
+        <v>46</v>
+      </c>
+      <c r="X3">
+        <v>1</v>
+      </c>
+      <c r="Y3">
+        <v>2</v>
+      </c>
+      <c r="Z3">
+        <v>3</v>
+      </c>
+      <c r="AA3">
+        <v>4</v>
+      </c>
+      <c r="AB3">
+        <v>5</v>
+      </c>
+      <c r="AC3">
+        <v>6</v>
+      </c>
+      <c r="AD3">
+        <v>7</v>
+      </c>
+      <c r="AE3">
+        <v>8</v>
+      </c>
+      <c r="AF3">
+        <v>9</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AH3">
+        <v>1</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ3">
+        <v>3</v>
+      </c>
+      <c r="AK3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="2" width="17.7109375" customWidth="1"/>
+    <col min="1" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="4" width="18.7109375" customWidth="1"/>
+    <col min="1" max="5" width="23.7109375" customWidth="1"/>
+    <col min="1" max="6" width="19.7109375" customWidth="1"/>
+    <col min="1" max="7" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" t="s">
+        <v>56</v>
+      </c>
+      <c r="G5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" t="s">
+        <v>56</v>
+      </c>
+      <c r="G7">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>